<commit_message>
Changed mosfet and layout of torpedo driver circuit
</commit_message>
<xml_diff>
--- a/dropper_torpedo/dropper_torpedo_BOM.xlsx
+++ b/dropper_torpedo/dropper_torpedo_BOM.xlsx
@@ -464,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +531,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G11" si="0">F3*E3</f>
+        <f t="shared" ref="G3:G12" si="0">F3*E3</f>
         <v>6.84</v>
       </c>
     </row>
@@ -697,6 +697,18 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added LED driver mosfet
</commit_message>
<xml_diff>
--- a/dropper_torpedo/dropper_torpedo_BOM.xlsx
+++ b/dropper_torpedo/dropper_torpedo_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Power Board V1.2: Bill of Materials</t>
   </si>
@@ -77,15 +77,6 @@
     <t>http://www.on-shore.com/wp-content/uploads/2015/09/osttcxx2162.pdf</t>
   </si>
   <si>
-    <t>MOSFET N-CH 55V 3.8A SOT223</t>
-  </si>
-  <si>
-    <t>http://www.infineon.com/dgdl/irll2705pbf.pdf?fileId=5546d462533600a401535664653425db</t>
-  </si>
-  <si>
-    <t>IRLL2705TRPBF</t>
-  </si>
-  <si>
     <t>LED GREEN CLEAR 1206 SMD</t>
   </si>
   <si>
@@ -114,6 +105,24 @@
   </si>
   <si>
     <t>EXB-V8V103JV</t>
+  </si>
+  <si>
+    <t>IRL6372TRPBF</t>
+  </si>
+  <si>
+    <t>MOSFET 2N-CH 30V 8.1A 8SOIC</t>
+  </si>
+  <si>
+    <t>http://www.infineon.com/dgdl/irl6372pbf.pdf?fileId=5546d462533600a401535660046e2579</t>
+  </si>
+  <si>
+    <t>SI4896DY-T1-E3</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 80V 6.7A 8-SOIC</t>
+  </si>
+  <si>
+    <t>http://www.vishay.com/docs/71300/71300.pdf</t>
   </si>
 </sst>
 </file>
@@ -464,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,189 +525,199 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1">
-        <v>1.1399999999999999</v>
+        <v>2.37</v>
       </c>
       <c r="F3" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G12" si="0">F3*E3</f>
-        <v>6.84</v>
+        <f t="shared" ref="G3:G13" si="0">F3*E3</f>
+        <v>4.74</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E4" s="1">
-        <v>0.53</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="F4" s="1">
         <v>2</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="0"/>
-        <v>1.06</v>
+        <f>F4*E4</f>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
-        <v>0.74</v>
+        <v>0.53</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>1.48</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1">
-        <v>1.08</v>
+        <v>0.74</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>2.16</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E7" s="1">
-        <v>0.46</v>
+        <v>1.08</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.92</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="3">
-        <v>39281043</v>
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E8" s="1">
-        <v>1.04</v>
+        <v>0.46</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>1.04</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="C9" s="3">
+        <v>39281043</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1">
-        <v>0.14000000000000001</v>
+        <v>1.04</v>
       </c>
       <c r="F9" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.56000000000000005</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E10" s="1">
         <v>0.14000000000000001</v>
       </c>
       <c r="F10" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0.28000000000000003</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -713,21 +732,34 @@
         <v>0</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="D6" r:id="rId4"/>
-    <hyperlink ref="D7" r:id="rId5"/>
-    <hyperlink ref="D8" r:id="rId6"/>
-    <hyperlink ref="D9" r:id="rId7"/>
-    <hyperlink ref="D10" r:id="rId8"/>
+    <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="D6" r:id="rId3"/>
+    <hyperlink ref="D7" r:id="rId4"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="D9" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="D11" r:id="rId8"/>
+    <hyperlink ref="D4" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed LED driver; Added servo connectors
</commit_message>
<xml_diff>
--- a/dropper_torpedo/dropper_torpedo_BOM.xlsx
+++ b/dropper_torpedo/dropper_torpedo_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Power Board V1.2: Bill of Materials</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>http://www.vishay.com/docs/71300/71300.pdf</t>
+  </si>
+  <si>
+    <t>http://www.on-shore.com/wp-content/uploads/2015/09/ostvnxxa150.pdf</t>
+  </si>
+  <si>
+    <t>OSTVN05A150</t>
+  </si>
+  <si>
+    <t>CONN TERM BLOCK 2.54MM 5POS PCB</t>
   </si>
 </sst>
 </file>
@@ -473,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +549,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G13" si="0">F3*E3</f>
+        <f t="shared" ref="G3:G15" si="0">F3*E3</f>
         <v>4.74</v>
       </c>
     </row>
@@ -722,14 +731,24 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2.34</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
       <c r="G12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.34</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -739,7 +758,28 @@
       <c r="D13" s="2"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -758,8 +798,9 @@
     <hyperlink ref="D10" r:id="rId7"/>
     <hyperlink ref="D11" r:id="rId8"/>
     <hyperlink ref="D4" r:id="rId9"/>
+    <hyperlink ref="D12" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added top layer gnd plane; Fixed MOLEX 5566 footprint
</commit_message>
<xml_diff>
--- a/dropper_torpedo/dropper_torpedo_BOM.xlsx
+++ b/dropper_torpedo/dropper_torpedo_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
   <si>
     <t>Power Board V1.2: Bill of Materials</t>
   </si>
@@ -132,6 +132,189 @@
   </si>
   <si>
     <t>CONN TERM BLOCK 2.54MM 5POS PCB</t>
+  </si>
+  <si>
+    <t>Q1, Q2</t>
+  </si>
+  <si>
+    <t>Q3, Q4</t>
+  </si>
+  <si>
+    <t>D1, D2</t>
+  </si>
+  <si>
+    <t>U1, U2</t>
+  </si>
+  <si>
+    <t>TRM1, TRM2</t>
+  </si>
+  <si>
+    <t>LED1-5</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>R11-14</t>
+  </si>
+  <si>
+    <t>R19, R23</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>CL31B105KBHNNNE</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 50V X7R 1206</t>
+  </si>
+  <si>
+    <t>https://www.samsungsem.com/kr/support/product-search/mlcc/__icsFiles/afieldfile/2016/08/18/S_CL31B105KBHNNNE.pdf</t>
+  </si>
+  <si>
+    <t>C1-3</t>
+  </si>
+  <si>
+    <t>http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_7.pdf</t>
+  </si>
+  <si>
+    <t>RC1206FR-071KL</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>RC1206FR-07220RL</t>
+  </si>
+  <si>
+    <t>RES SMD 220 OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>RC1206FR-073KL</t>
+  </si>
+  <si>
+    <t>RES SMD 3K OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>RC1206FR-0710KL</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>RC1206FR-074K99L</t>
+  </si>
+  <si>
+    <t>RES SMD 4.99K OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>RC1206FR-07240RL</t>
+  </si>
+  <si>
+    <t>RC1206FR-072KL</t>
+  </si>
+  <si>
+    <t>RES SMD 240 OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>RES SMD 2K OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>RC1206FR-07576RL</t>
+  </si>
+  <si>
+    <t>RES SMD 576 OHM 1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R4,5</t>
+  </si>
+  <si>
+    <t>R7,8,22</t>
+  </si>
+  <si>
+    <t>R9,10</t>
+  </si>
+  <si>
+    <t>R15,16</t>
+  </si>
+  <si>
+    <t>R1,2</t>
+  </si>
+  <si>
+    <t>R3,4,9,10,17,18,23</t>
+  </si>
+  <si>
+    <t>PCA9685PW,118</t>
+  </si>
+  <si>
+    <t>IC LED DRIVER RGBA 28-TSSOP</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>http://www.nxp.com/documents/data_sheet/PCA9685.pdf</t>
+  </si>
+  <si>
+    <t>PPPC141LFBN-RC</t>
+  </si>
+  <si>
+    <t>CONN HEADER FMALE 14POS .1" GOLD</t>
+  </si>
+  <si>
+    <t>http://www.sullinscorp.com/drawings/78_P(N)PxCxxxLFBN-RC,_10492-H.pdf</t>
+  </si>
+  <si>
+    <t>M20-9980345</t>
+  </si>
+  <si>
+    <t>https://cdn.harwin.com/pdfs/M20-998.pdf</t>
+  </si>
+  <si>
+    <t>DIL VERTICAL PC TAIL PIN HEADER 2x3</t>
+  </si>
+  <si>
+    <t>M20-9980445</t>
+  </si>
+  <si>
+    <t>DIL VERTICAL PC TAIL PIN HEADER 2x4</t>
+  </si>
+  <si>
+    <t>M20-9990445</t>
+  </si>
+  <si>
+    <t>https://cdn.harwin.com/pdfs/M20-999.pdf</t>
+  </si>
+  <si>
+    <t>SIL VERTICAL PC TAIL PIN HEADER 1x4</t>
+  </si>
+  <si>
+    <t>M20-9990245</t>
+  </si>
+  <si>
+    <t>SIL VERTICAL PC TAIL PIN HEADER 1x2</t>
+  </si>
+  <si>
+    <t>JP9</t>
+  </si>
+  <si>
+    <t>JP1-7, 10, 11</t>
+  </si>
+  <si>
+    <t>Teensy 3.2</t>
+  </si>
+  <si>
+    <t>JP8</t>
+  </si>
+  <si>
+    <t>JP12</t>
   </si>
 </sst>
 </file>
@@ -482,15 +665,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="48" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
     <col min="4" max="4" width="31.85546875" customWidth="1"/>
@@ -532,7 +715,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>31</v>
       </c>
@@ -554,7 +739,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
@@ -576,7 +763,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -598,7 +787,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
@@ -620,7 +811,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
@@ -642,7 +835,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
@@ -664,7 +859,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
@@ -686,7 +883,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
@@ -708,7 +907,9 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
@@ -730,7 +931,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
@@ -752,35 +955,374 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
       <c r="G14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.7E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
       <c r="G15" s="1">
         <f t="shared" si="0"/>
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" ref="G16:G23" si="1">F16*E16</f>
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14100000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="1"/>
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="1"/>
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="1"/>
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <v>4</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="1"/>
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="1"/>
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1.28</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="1"/>
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="F24" s="1">
+        <v>10</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" ref="G24:G28" si="2">F24*E24</f>
+        <v>3.4799999999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="2"/>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="2"/>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -799,8 +1341,22 @@
     <hyperlink ref="D11" r:id="rId8"/>
     <hyperlink ref="D4" r:id="rId9"/>
     <hyperlink ref="D12" r:id="rId10"/>
+    <hyperlink ref="D13" r:id="rId11"/>
+    <hyperlink ref="D14" r:id="rId12"/>
+    <hyperlink ref="D15" r:id="rId13"/>
+    <hyperlink ref="D16" r:id="rId14"/>
+    <hyperlink ref="D17" r:id="rId15"/>
+    <hyperlink ref="D18" r:id="rId16"/>
+    <hyperlink ref="D19" r:id="rId17"/>
+    <hyperlink ref="D20" r:id="rId18"/>
+    <hyperlink ref="D21" r:id="rId19"/>
+    <hyperlink ref="D23" r:id="rId20"/>
+    <hyperlink ref="D24" r:id="rId21"/>
+    <hyperlink ref="D25" r:id="rId22"/>
+    <hyperlink ref="D26" r:id="rId23"/>
+    <hyperlink ref="D27" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added CAN bus transceiver
</commit_message>
<xml_diff>
--- a/dropper_torpedo/dropper_torpedo_BOM.xlsx
+++ b/dropper_torpedo/dropper_torpedo_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="100">
   <si>
     <t>Power Board V1.2: Bill of Materials</t>
   </si>
@@ -315,6 +315,15 @@
   </si>
   <si>
     <t>JP12</t>
+  </si>
+  <si>
+    <t>TCAN1042HVDRQ1</t>
+  </si>
+  <si>
+    <t>IC TXRX CAN FAULT PROT 8SOIC</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/tcan1042hgv-q1.pdf</t>
   </si>
 </sst>
 </file>
@@ -665,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,7 +1247,7 @@
         <v>10</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" ref="G24:G28" si="2">F24*E24</f>
+        <f t="shared" ref="G24:G29" si="2">F24*E24</f>
         <v>3.4799999999999995</v>
       </c>
     </row>
@@ -1316,12 +1325,34 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
       <c r="G28" s="1">
+        <f t="shared" si="2"/>
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1355,8 +1386,9 @@
     <hyperlink ref="D25" r:id="rId22"/>
     <hyperlink ref="D26" r:id="rId23"/>
     <hyperlink ref="D27" r:id="rId24"/>
+    <hyperlink ref="D28" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId25"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified CAN bus transceiver layout; Updated BOM, CAM files
</commit_message>
<xml_diff>
--- a/dropper_torpedo/dropper_torpedo_BOM.xlsx
+++ b/dropper_torpedo/dropper_torpedo_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="108">
   <si>
     <t>Power Board V1.2: Bill of Materials</t>
   </si>
@@ -155,12 +155,6 @@
     <t>X1</t>
   </si>
   <si>
-    <t>R11-14</t>
-  </si>
-  <si>
-    <t>R19, R23</t>
-  </si>
-  <si>
     <t>X2</t>
   </si>
   <si>
@@ -173,9 +167,6 @@
     <t>https://www.samsungsem.com/kr/support/product-search/mlcc/__icsFiles/afieldfile/2016/08/18/S_CL31B105KBHNNNE.pdf</t>
   </si>
   <si>
-    <t>C1-3</t>
-  </si>
-  <si>
     <t>http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_7.pdf</t>
   </si>
   <si>
@@ -185,12 +176,6 @@
     <t>RES SMD 1K OHM 1% 1/4W 1206</t>
   </si>
   <si>
-    <t>RC1206FR-07220RL</t>
-  </si>
-  <si>
-    <t>RES SMD 220 OHM 1% 1/4W 1206</t>
-  </si>
-  <si>
     <t>RC1206FR-073KL</t>
   </si>
   <si>
@@ -221,9 +206,6 @@
     <t>RES SMD 2K OHM 1% 1/4W 1206</t>
   </si>
   <si>
-    <t>R20</t>
-  </si>
-  <si>
     <t>RC1206FR-07576RL</t>
   </si>
   <si>
@@ -233,24 +215,9 @@
     <t>R21</t>
   </si>
   <si>
-    <t>R4,5</t>
-  </si>
-  <si>
-    <t>R7,8,22</t>
-  </si>
-  <si>
-    <t>R9,10</t>
-  </si>
-  <si>
-    <t>R15,16</t>
-  </si>
-  <si>
     <t>R1,2</t>
   </si>
   <si>
-    <t>R3,4,9,10,17,18,23</t>
-  </si>
-  <si>
     <t>PCA9685PW,118</t>
   </si>
   <si>
@@ -287,36 +254,21 @@
     <t>DIL VERTICAL PC TAIL PIN HEADER 2x4</t>
   </si>
   <si>
-    <t>M20-9990445</t>
-  </si>
-  <si>
     <t>https://cdn.harwin.com/pdfs/M20-999.pdf</t>
   </si>
   <si>
-    <t>SIL VERTICAL PC TAIL PIN HEADER 1x4</t>
-  </si>
-  <si>
     <t>M20-9990245</t>
   </si>
   <si>
     <t>SIL VERTICAL PC TAIL PIN HEADER 1x2</t>
   </si>
   <si>
-    <t>JP9</t>
-  </si>
-  <si>
-    <t>JP1-7, 10, 11</t>
-  </si>
-  <si>
     <t>Teensy 3.2</t>
   </si>
   <si>
     <t>JP8</t>
   </si>
   <si>
-    <t>JP12</t>
-  </si>
-  <si>
     <t>TCAN1042HVDRQ1</t>
   </si>
   <si>
@@ -324,6 +276,78 @@
   </si>
   <si>
     <t>http://www.ti.com/lit/ds/symlink/tcan1042hgv-q1.pdf</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>RC0805FR-07220RL</t>
+  </si>
+  <si>
+    <t>RES SMD 220 OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R14-17</t>
+  </si>
+  <si>
+    <t>R20,24</t>
+  </si>
+  <si>
+    <t>CL21B106KOQNNNG</t>
+  </si>
+  <si>
+    <t>http://www.samsungsem.com/kr/support/product-search/mlcc/CL21B106KOQNNNG.jsp</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 16V X7R 0805</t>
+  </si>
+  <si>
+    <t>C1,2</t>
+  </si>
+  <si>
+    <t>C3,4,5</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R5,6</t>
+  </si>
+  <si>
+    <t>R7,8,23</t>
+  </si>
+  <si>
+    <t>R9,R10</t>
+  </si>
+  <si>
+    <t>R12,13</t>
+  </si>
+  <si>
+    <t>R3,4,18,19</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RC0805FR-071KL</t>
+  </si>
+  <si>
+    <t>JP11</t>
+  </si>
+  <si>
+    <t>JP1-7,9,10</t>
+  </si>
+  <si>
+    <t>CON1</t>
+  </si>
+  <si>
+    <t>CONN HEADER 2POS 4.2MM VERT TIN</t>
+  </si>
+  <si>
+    <t>http://www.molex.com/pdm_docs/sd/039281023_sd.pdf</t>
   </si>
 </sst>
 </file>
@@ -674,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +767,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G15" si="0">F3*E3</f>
+        <f t="shared" ref="G3:G16" si="0">F3*E3</f>
         <v>4.74</v>
       </c>
     </row>
@@ -869,7 +893,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>20</v>
@@ -893,7 +917,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>22</v>
@@ -917,7 +941,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>25</v>
@@ -965,64 +989,64 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="E13" s="1">
         <v>0.26</v>
       </c>
       <c r="F13" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="0"/>
-        <v>0.78</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="E14" s="1">
-        <v>4.7E-2</v>
+        <v>0.39</v>
       </c>
       <c r="F14" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="0"/>
-        <v>4.7E-2</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E15" s="1">
         <v>4.7E-2</v>
@@ -1037,88 +1061,88 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E16" s="1">
         <v>4.7E-2</v>
       </c>
       <c r="F16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" ref="G16:G23" si="1">F16*E16</f>
-        <v>9.4E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.7E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E17" s="1">
         <v>4.7E-2</v>
       </c>
       <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" ref="G17:G25" si="1">F17*E17</f>
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F18" s="1">
         <v>3</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G18" s="1">
         <f t="shared" si="1"/>
         <v>0.14100000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="1">
-        <v>4.7E-2</v>
-      </c>
-      <c r="F18" s="1">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1">
-        <f t="shared" si="1"/>
-        <v>9.4E-2</v>
-      </c>
-    </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E19" s="1">
         <v>4.7E-2</v>
@@ -1133,228 +1157,266 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E20" s="1">
-        <v>4.7E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="F20" s="1">
         <v>2</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="1"/>
-        <v>9.4E-2</v>
+        <v>6.2E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E21" s="1">
         <v>4.7E-2</v>
       </c>
       <c r="F21" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="1"/>
-        <v>0.188</v>
+        <v>9.4E-2</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="E22" s="1">
-        <v>3.3</v>
+        <v>4.7E-2</v>
       </c>
       <c r="F22" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="1"/>
-        <v>3.3</v>
+        <v>0.188</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="E23" s="1">
-        <v>1.28</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="F23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="1"/>
-        <v>2.56</v>
+        <v>3.4000000000000002E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B24" s="3" t="s">
         <v>84</v>
       </c>
+      <c r="B24" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="C24" s="3" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E24" s="1">
-        <v>0.34799999999999998</v>
+        <v>3.3</v>
       </c>
       <c r="F24" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" ref="G24:G29" si="2">F24*E24</f>
-        <v>3.4799999999999995</v>
+        <f t="shared" si="1"/>
+        <v>3.3</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E25" s="1">
+        <v>1.28</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="1"/>
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="F26" s="1">
+        <v>9</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" ref="G26:G30" si="2">F26*E26</f>
+        <v>3.1319999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="1">
         <v>0.48</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F27" s="1">
         <v>1</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G27" s="1">
         <f t="shared" si="2"/>
         <v>0.48</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="F26" s="1">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F28" s="1">
         <v>1</v>
       </c>
-      <c r="G26" s="1">
-        <f t="shared" si="2"/>
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="F27" s="1">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1">
+      <c r="G28" s="1">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E28" s="1">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="1">
         <v>2.0499999999999998</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F29" s="1">
         <v>1</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G29" s="1">
         <f t="shared" si="2"/>
         <v>2.0499999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="3">
+        <v>39281023</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.83</v>
       </c>
     </row>
   </sheetData>
@@ -1373,22 +1435,24 @@
     <hyperlink ref="D4" r:id="rId9"/>
     <hyperlink ref="D12" r:id="rId10"/>
     <hyperlink ref="D13" r:id="rId11"/>
-    <hyperlink ref="D14" r:id="rId12"/>
-    <hyperlink ref="D15" r:id="rId13"/>
-    <hyperlink ref="D16" r:id="rId14"/>
-    <hyperlink ref="D17" r:id="rId15"/>
-    <hyperlink ref="D18" r:id="rId16"/>
-    <hyperlink ref="D19" r:id="rId17"/>
-    <hyperlink ref="D20" r:id="rId18"/>
-    <hyperlink ref="D21" r:id="rId19"/>
-    <hyperlink ref="D23" r:id="rId20"/>
-    <hyperlink ref="D24" r:id="rId21"/>
-    <hyperlink ref="D25" r:id="rId22"/>
-    <hyperlink ref="D26" r:id="rId23"/>
-    <hyperlink ref="D27" r:id="rId24"/>
-    <hyperlink ref="D28" r:id="rId25"/>
+    <hyperlink ref="D15" r:id="rId12"/>
+    <hyperlink ref="D16" r:id="rId13"/>
+    <hyperlink ref="D17" r:id="rId14"/>
+    <hyperlink ref="D18" r:id="rId15"/>
+    <hyperlink ref="D19" r:id="rId16"/>
+    <hyperlink ref="D20" r:id="rId17"/>
+    <hyperlink ref="D21" r:id="rId18"/>
+    <hyperlink ref="D22" r:id="rId19"/>
+    <hyperlink ref="D25" r:id="rId20"/>
+    <hyperlink ref="D26" r:id="rId21"/>
+    <hyperlink ref="D27" r:id="rId22"/>
+    <hyperlink ref="D28" r:id="rId23"/>
+    <hyperlink ref="D29" r:id="rId24"/>
+    <hyperlink ref="D14" r:id="rId25"/>
+    <hyperlink ref="D23" r:id="rId26"/>
+    <hyperlink ref="D30" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId26"/>
+  <pageSetup orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improved CAN transceiver design; Modified layout, traces;
</commit_message>
<xml_diff>
--- a/dropper_torpedo/dropper_torpedo_BOM.xlsx
+++ b/dropper_torpedo/dropper_torpedo_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="117">
   <si>
     <t>Shematic Reference Number</t>
   </si>
@@ -185,12 +185,6 @@
     <t>RES SMD 10K OHM 1% 1/4W 1206</t>
   </si>
   <si>
-    <t>RC1206FR-074K99L</t>
-  </si>
-  <si>
-    <t>RES SMD 4.99K OHM 1% 1/4W 1206</t>
-  </si>
-  <si>
     <t>RC1206FR-07240RL</t>
   </si>
   <si>
@@ -209,9 +203,6 @@
     <t>RES SMD 576 OHM 1% 1/4W 1206</t>
   </si>
   <si>
-    <t>R21</t>
-  </si>
-  <si>
     <t>R1,2</t>
   </si>
   <si>
@@ -287,9 +278,6 @@
     <t>R14-17</t>
   </si>
   <si>
-    <t>R20,24</t>
-  </si>
-  <si>
     <t>CL21B106KOQNNNG</t>
   </si>
   <si>
@@ -305,27 +293,9 @@
     <t>C3,4,5</t>
   </si>
   <si>
-    <t>R22</t>
-  </si>
-  <si>
     <t>R5,6</t>
   </si>
   <si>
-    <t>R7,8,23</t>
-  </si>
-  <si>
-    <t>R9,R10</t>
-  </si>
-  <si>
-    <t>R12,13</t>
-  </si>
-  <si>
-    <t>R3,4,18,19</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
     <t>RES SMD 1K OHM 1% 1/8W 0805</t>
   </si>
   <si>
@@ -338,9 +308,6 @@
     <t>JP1-7,9,10</t>
   </si>
   <si>
-    <t>CON1</t>
-  </si>
-  <si>
     <t>CONN HEADER 2POS 4.2MM VERT TIN</t>
   </si>
   <si>
@@ -360,6 +327,54 @@
   </si>
   <si>
     <t>Torpedo Board V3: Bill of Materials</t>
+  </si>
+  <si>
+    <t>R22,26</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R7,8,25</t>
+  </si>
+  <si>
+    <t>RC0805FR-074K99L</t>
+  </si>
+  <si>
+    <t>http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_8.pdf</t>
+  </si>
+  <si>
+    <t>RES SMD 4.99K OHM 1% 1/4W 0805</t>
+  </si>
+  <si>
+    <t>R9-12</t>
+  </si>
+  <si>
+    <t>R18, 19</t>
+  </si>
+  <si>
+    <t>R3,4,20,21</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>CON3</t>
+  </si>
+  <si>
+    <t>CON1,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM03B-GHS-TB </t>
+  </si>
+  <si>
+    <t>http://www.jst-mfg.com/product/pdf/eng/eGH.pdf</t>
+  </si>
+  <si>
+    <t>CONN HEADER GH SIDE 3POS 1.25MM</t>
   </si>
 </sst>
 </file>
@@ -710,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +742,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -929,7 +944,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -953,7 +968,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
@@ -1001,7 +1016,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>44</v>
@@ -1025,16 +1040,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E14" s="1">
         <v>0.39</v>
@@ -1049,13 +1064,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>46</v>
@@ -1073,13 +1088,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>46</v>
@@ -1097,7 +1112,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>48</v>
@@ -1121,13 +1136,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>46</v>
@@ -1145,37 +1160,37 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="E19" s="1">
-        <v>4.7E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="F19" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="1"/>
-        <v>9.4E-2</v>
+        <v>0.124</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>46</v>
@@ -1193,7 +1208,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>50</v>
@@ -1217,7 +1232,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>52</v>
@@ -1241,13 +1256,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>46</v>
@@ -1265,16 +1280,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="E24" s="1">
         <v>3.3</v>
@@ -1289,16 +1304,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E25" s="1">
         <v>1.28</v>
@@ -1313,16 +1328,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E26" s="1">
         <v>0.34799999999999998</v>
@@ -1331,22 +1346,22 @@
         <v>9</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" ref="G26:G30" si="2">F26*E26</f>
+        <f t="shared" ref="G26:G29" si="2">F26*E26</f>
         <v>3.1319999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E27" s="1">
         <v>0.48</v>
@@ -1361,16 +1376,16 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E28" s="1">
         <v>0.2</v>
@@ -1385,16 +1400,16 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E29" s="1">
         <v>2.0499999999999998</v>
@@ -1409,16 +1424,16 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C30" s="3">
         <v>39281023</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="E30" s="1">
         <v>0.83</v>
@@ -1427,31 +1442,55 @@
         <v>1</v>
       </c>
       <c r="G30" s="1">
-        <f t="shared" si="2"/>
+        <f>F30*E30</f>
         <v>0.83</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="E31" s="1">
-        <v>8.3000000000000004E-2</v>
+        <v>0.68</v>
       </c>
       <c r="F31" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" ref="G31" si="3">F31*E31</f>
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F32" s="1">
+        <v>9</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" ref="G32" si="4">F32*E32</f>
         <v>0.747</v>
       </c>
     </row>
@@ -1487,9 +1526,10 @@
     <hyperlink ref="D14" r:id="rId25"/>
     <hyperlink ref="D23" r:id="rId26"/>
     <hyperlink ref="D30" r:id="rId27"/>
-    <hyperlink ref="D31" r:id="rId28"/>
+    <hyperlink ref="D32" r:id="rId28"/>
+    <hyperlink ref="D31" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed JST connectors from 1.5mm to 2.0mm pitch
</commit_message>
<xml_diff>
--- a/dropper_torpedo/dropper_torpedo_BOM.xlsx
+++ b/dropper_torpedo/dropper_torpedo_BOM.xlsx
@@ -368,13 +368,13 @@
     <t>CON1,2</t>
   </si>
   <si>
-    <t xml:space="preserve">SM03B-GHS-TB </t>
-  </si>
-  <si>
-    <t>http://www.jst-mfg.com/product/pdf/eng/eGH.pdf</t>
-  </si>
-  <si>
-    <t>CONN HEADER GH SIDE 3POS 1.25MM</t>
+    <t>S3B-PH-SM4-TB</t>
+  </si>
+  <si>
+    <t>CONN HEADER PH SIDE 3POS 2MM SMD</t>
+  </si>
+  <si>
+    <t>http://www.jst-mfg.com/product/pdf/eng/ePH.pdf</t>
   </si>
 </sst>
 </file>
@@ -728,7 +728,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,23 +1451,23 @@
         <v>113</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>114</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E31" s="1">
-        <v>0.68</v>
+        <v>0.96</v>
       </c>
       <c r="F31" s="1">
         <v>2</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" ref="G31" si="3">F31*E31</f>
-        <v>1.36</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed CAN bus connector back to JST GH series due to long Digikey lead time for PH crimp connectors
</commit_message>
<xml_diff>
--- a/dropper_torpedo/dropper_torpedo_BOM.xlsx
+++ b/dropper_torpedo/dropper_torpedo_BOM.xlsx
@@ -368,13 +368,13 @@
     <t>CON1,2</t>
   </si>
   <si>
-    <t>S3B-PH-SM4-TB</t>
-  </si>
-  <si>
-    <t>CONN HEADER PH SIDE 3POS 2MM SMD</t>
-  </si>
-  <si>
-    <t>http://www.jst-mfg.com/product/pdf/eng/ePH.pdf</t>
+    <t>SM03B-GHS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>CONN HEADER GH SIDE 3POS 1.25MM</t>
+  </si>
+  <si>
+    <t>http://www.jst-mfg.com/product/pdf/eng/eGH.pdf</t>
   </si>
 </sst>
 </file>
@@ -728,7 +728,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1460,14 +1460,14 @@
         <v>116</v>
       </c>
       <c r="E31" s="1">
-        <v>0.96</v>
+        <v>0.68</v>
       </c>
       <c r="F31" s="1">
         <v>2</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" ref="G31" si="3">F31*E31</f>
-        <v>1.92</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>